<commit_message>
ajustes migração final e consolidação cabl
</commit_message>
<xml_diff>
--- a/consolidacao/pedidos/CABL_pedidos.xlsx
+++ b/consolidacao/pedidos/CABL_pedidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,10 +490,10 @@
         <v>64</v>
       </c>
       <c r="E2" t="n">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F2" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -504,7 +504,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>30.07.705</t>
+          <t>30.07.1462</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -514,28 +514,28 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ADOÇANTE ASPECTO FISICO LÍQUIDO TRANSPARENTE, INGREDIENTES SUCRALOSEPRAZO VAL. 1 ANO, TIPO DIETÉTICO, CARACT. ADICIONAIS BICO DOSADOR MARCA GOLD.</t>
+          <t>Açucar cristal 1KG</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>30.07.835</t>
+          <t>30.07.705</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -545,21 +545,21 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>AÇÚCAR, TIPO CRISTAL, PACOTE DE 1KG.</t>
+          <t>ADOÇANTE ASPECTO FISICO LÍQUIDO TRANSPARENTE, INGREDIENTES SUCRALOSEPRAZO VAL. 1 ANO, TIPO DIETÉTICO, CARACT. ADICIONAIS BICO DOSADOR MARCA GOLD.</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E4" t="n">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
-        <v>-49</v>
+        <v>0</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>30.16.1096</t>
+          <t>30.16.1139</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -669,17 +669,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>COLCHETE (BAILARINA), Nº 15, COMPRIMENTO DA HASTE 10CM, DIÂMETRO DA CABEÇA 14MM, PARA FIXAR ATÉ 450 FOLHAS, MATERIAL LATÃO, CAIXA COM 72 UNIDADES.</t>
+          <t>CLIPE DE METAL TAM. 2/0, CX C/ 100 UND.</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E8" t="n">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="F8" t="n">
-        <v>-6</v>
+        <v>-79</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -690,7 +690,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>30.16.1139</t>
+          <t>30.16.1178</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -700,28 +700,28 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CLIPE DE METAL TAM. 2/0, CX C/ 100 UND.</t>
+          <t>APAGADOR PARA QUADRO BRANCO, BASE FELTRO, CORPO PLÁSTICO, 15CMX6CM.</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="E9" t="n">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="F9" t="n">
-        <v>-80</v>
+        <v>0</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>30.16.1178</t>
+          <t>30.16.1183</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -731,28 +731,28 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>APAGADOR PARA QUADRO BRANCO, BASE FELTRO, CORPO PLÁSTICO, 15CMX6CM.</t>
+          <t>PAPEL A4, TIPO RECICLADO, RESMA (500 FLS).</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="E10" t="n">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>30.16.1183</t>
+          <t>30.16.1189</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -762,17 +762,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PAPEL A4, TIPO RECICLADO, RESMA (500 FLS).</t>
+          <t>PASTA SANFONADA, MATERIAL PLÁSTICO/PVC, COM 12 DIVISÕES, TAMANHO 235MM X 320MM X 30MM, COR FUMÊ, FECHAMENTO COM ELÁSTICO.</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="E11" t="n">
-        <v>168</v>
+        <v>43</v>
       </c>
       <c r="F11" t="n">
-        <v>-28</v>
+        <v>-24</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -783,7 +783,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>30.16.1189</t>
+          <t>30.16.1296</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -793,28 +793,28 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>PASTA SANFONADA, MATERIAL PLÁSTICO/PVC, COM 12 DIVISÕES, TAMANHO 235MM X 320MM X 30MM, COR FUMÊ, FECHAMENTO COM ELÁSTICO.</t>
+          <t>Papel A3 90g</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E12" t="n">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F12" t="n">
-        <v>-24</v>
+        <v>0</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>30.16.129</t>
+          <t>30.16.1389</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -824,28 +824,28 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>PINCEL ATÔMICO (CORES VARIADAS)</t>
+          <t>GRAMPO GRAMPEADOR, MATERIAL METAL, TRATAMENTO SUPERFICIAL NIQUELADO, TAMANHO 23/8</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>pedido no suap</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>30.16.1296</t>
+          <t>30.16.1461</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -855,28 +855,28 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Papel A3 90g</t>
+          <t>PAPEL CREPOM, MATERIAL CELULOSE VEGETAL, 18 G/M2, COMPRIMENTO 2 M, LARGURA 48 CM, COR VARIADA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>8</v>
+        <v>94</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>30.16.1364</t>
+          <t>30.16.1516</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -886,28 +886,28 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>FITA ADESIVA CREPE 50X50 COR BRANCA.</t>
+          <t>CADERNO, MATERIAL CELULOSE VEGETAL, MATERIAL CAPA PLÁSTICO, APRESENTAÇÃO ESPIRAL, 200 FLS, 280X205MM.</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E15" t="n">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="F15" t="n">
-        <v>-74</v>
+        <v>0</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>30.16.1389</t>
+          <t>30.16.1523</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -917,28 +917,28 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>GRAMPO GRAMPEADOR, MATERIAL METAL, TRATAMENTO SUPERFICIAL NIQUELADO, TAMANHO 23/8</t>
+          <t>SACO DOCUMENTO, MATERIAL PLÁSTICO TRANSPARENTE, CAPACIDADE FOLHAS 40 FL, COMPRIMENTO 330 MM, LARGURA 240 MM, NÚMERO FUROS SEM FUROS. PACOTE COM 50 UN.</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F16" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>30.16.1441</t>
+          <t>30.16.1694</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -948,17 +948,17 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>PINCEL MARCADOR PERMANENTE CD, MATERIAL PLÁSTICO, TIPO PONTA POLIÉSTER, COR TINTA PRETA, CARACTERÍSTICAS ADICIONAIS PONTA 2MM</t>
+          <t>PAPEL A4, MATERIAL PAPEL ALCALINO, COMPRIMENTO 297MM, LARGURA 210MM, GRAMATURA 75 G/M2, COR BRANCA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="E17" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F17" t="n">
-        <v>-41</v>
+        <v>-16</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -969,7 +969,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>30.16.1461</t>
+          <t>30.16.1716</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -979,28 +979,28 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>PAPEL CREPOM, MATERIAL CELULOSE VEGETAL, 18 G/M2, COMPRIMENTO 2 M, LARGURA 48 CM, COR VARIADA</t>
+          <t>Bloco recado , material reciclado, cor natural, largura 38 MM, comprimento 50 MM, características adicionais auto-adesiva.</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>pedido no suap</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>30.16.1516</t>
+          <t>30.16.1759</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1010,28 +1010,28 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>CADERNO, MATERIAL CELULOSE VEGETAL, MATERIAL CAPA PLÁSTICO, APRESENTAÇÃO ESPIRAL, 200 FLS, 280X205MM.</t>
+          <t>MINA GRAFITE, 0,9MM, CAIXA C/12.</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E19" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>30.16.1523</t>
+          <t>30.16.1941</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1041,14 +1041,14 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SACO DOCUMENTO, MATERIAL PLÁSTICO TRANSPARENTE, CAPACIDADE FOLHAS 40 FL, COMPRIMENTO 330 MM, LARGURA 240 MM, NÚMERO FUROS SEM FUROS. PACOTE COM 50 UN.</t>
+          <t>ETIQUETA ADESIVA (110mm x 75m) - ribbon - material 100% resina; com resistência a solventes e abrasão comprovada após teste no local; cor preta; filme base em poliéster; velocidade de impressão: até 10 polegadas/segundo; rolo 90 metros.</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1062,7 +1062,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>30.16.1694</t>
+          <t>30.16.1942</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1072,28 +1072,28 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>PAPEL A4, MATERIAL PAPEL ALCALINO, COMPRIMENTO 297MM, LARGURA 210MM, GRAMATURA 75 G/M2, COR BRANCA</t>
+          <t>ETIQUETA PARA IDENTIFICAÇÃO DE PATRIMÔNIO, TAMANHO 45mm DE LARGURA x 20mm DE ALTURA, CONFECCIONADA EM POLIÉSTER PRATA CROMO FOSCO, IMPRESSÃO CÓDIGO DE BARRA, 02 COLUNAS, ROLO COM 2000 ETIQUETAS. MARCA: ETIBRAS.</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E21" t="n">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="F21" t="n">
-        <v>-17</v>
+        <v>0</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>30.16.1716</t>
+          <t>30.16.1954</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1103,14 +1103,14 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Bloco recado , material reciclado, cor natural, largura 38 MM, comprimento 50 MM, características adicionais auto-adesiva.</t>
+          <t>BARBANTE ALGODÃO, QUANTIDADE FIOS 6 UNIDADES, ACABAMENTO SUPERFICIAL CRU.</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1124,7 +1124,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>30.16.1759</t>
+          <t>30.16.1959</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1134,28 +1134,28 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MINA GRAFITE, 0,9MM, CAIXA C/12.</t>
+          <t>CALCULADORA ELETRÔNICA DE BOLSO 8 DÍGITOS. POSSUI VISOR DE LCD, CALCULA RAIZ QUADRADA, PORCENTAGEM, ALÉM DAS QUATRO OPERAÇÕES BÁSICAS. POSSUI MEMÓRIA DE DESLIGAMENTO AUTOMÁTICO, COM FUNCIONAMENTO A PILHA AA OU AAA 1,5V ENERGIA SOLAR MARCA: KENKO</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="E23" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>30.16.1941</t>
+          <t>30.16.1976</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1165,28 +1165,28 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>ETIQUETA ADESIVA (110mm x 75m) - ribbon - material 100% resina; com resistência a solventes e abrasão comprovada após teste no local; cor preta; filme base em poliéster; velocidade de impressão: até 10 polegadas/segundo; rolo 90 metros.</t>
+          <t>Clipe de metal. Tamanho: 6/0; caixa com 100 unidades.</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F24" t="n">
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>pedido no suap</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>30.16.1942</t>
+          <t>30.16.1985</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1196,28 +1196,28 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ETIQUETA PARA IDENTIFICAÇÃO DE PATRIMÔNIO, TAMANHO 45mm DE LARGURA x 20mm DE ALTURA, CONFECCIONADA EM POLIÉSTER PRATA CROMO FOSCO, IMPRESSÃO CÓDIGO DE BARRA, 02 COLUNAS, ROLO COM 2000 ETIQUETAS. MARCA: ETIBRAS.</t>
+          <t>Fita adesiva, material crepe, tipo monoface, largura 50 mm cumprimento 50 m, cor branca, aplicação multi uso, Marca : altape.</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E25" t="n">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>-70</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>30.16.1959</t>
+          <t>30.16.1991</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1227,28 +1227,28 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CALCULADORA ELETRÔNICA DE BOLSO 8 DÍGITOS. POSSUI VISOR DE LCD, CALCULA RAIZ QUADRADA, PORCENTAGEM, ALÉM DAS QUATRO OPERAÇÕES BÁSICAS. POSSUI MEMÓRIA DE DESLIGAMENTO AUTOMÁTICO, COM FUNCIONAMENTO A PILHA AA OU AAA 1,5V ENERGIA SOLAR MARCA: KENKO</t>
+          <t>Mina grafite. Material: grafita; Diâmetro: 0,70 mm; Comprimento: 60 mm; Dureza. B. Marca: CIS.</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>192</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>-185</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>30.16.1976</t>
+          <t>30.16.1997</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1258,17 +1258,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Clipe de metal. Tamanho: 6/0; caixa com 100 unidades.</t>
+          <t>Fita sinalização, material plástico, largura 70 mm, cor preta e amarela, aplicação sinalização de advertência, características adicionais formato cores em diagonal, zebrada.</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E27" t="n">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="F27" t="n">
-        <v>-2</v>
+        <v>-47</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>30.16.1991</t>
+          <t>30.16.2007</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1289,17 +1289,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Mina grafite. Material: grafita; Diâmetro: 0,70 mm; Comprimento: 60 mm; Dureza. B. Marca: CIS.</t>
+          <t>Marcador de página, cor diversas, características adicionais, adesivos reposicionáveis, setas, neon, marca kas.</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E28" t="n">
-        <v>209</v>
+        <v>22</v>
       </c>
       <c r="F28" t="n">
-        <v>-202</v>
+        <v>-14</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1310,7 +1310,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>30.16.2007</t>
+          <t>30.16.2019</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1320,28 +1320,28 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Marcador de página, cor diversas, características adicionais, adesivos reposicionáveis, setas, neon, marca kas.</t>
+          <t>Pistola aplicadora de cola quente. Bivoltagem: 110/220 V; 40 Watts; ponta com isolante térmico; para refil de 11 a 12 mm de diâmetro. Marca: Jocar.</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E29" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>-14</v>
+        <v>0</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>30.16.2019</t>
+          <t>30.16.2021</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1351,28 +1351,28 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Pistola aplicadora de cola quente. Bivoltagem: 110/220 V; 40 Watts; ponta com isolante térmico; para refil de 11 a 12 mm de diâmetro. Marca: Jocar.</t>
+          <t>Cola. Composição: silicone; incolor; tipo bastão. Marca: Jocar.</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E30" t="n">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>-33</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>30.16.2021</t>
+          <t>30.16.2025</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1382,28 +1382,28 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Cola. Composição: silicone; incolor; tipo bastão. Marca: Jocar.</t>
+          <t>Copo descartável, capacidade 50 mL, pacote com 100 UND.</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>24</v>
+        <v>169</v>
       </c>
       <c r="E31" t="n">
-        <v>60</v>
+        <v>164</v>
       </c>
       <c r="F31" t="n">
-        <v>-36</v>
+        <v>5</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>30.16.2025</t>
+          <t>30.16.2061</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1413,28 +1413,28 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Copo descartável, capacidade 50 mL, pacote com 100 UND.</t>
+          <t>Calculadora eletrônica de mesa, com 12 dígitos, alimentação com bateria HR1130 ou célula solar. Marca: Kenko.</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>169</v>
+        <v>13</v>
       </c>
       <c r="E32" t="n">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="F32" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>30.16.2061</t>
+          <t>30.16.2125</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1444,21 +1444,21 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Calculadora eletrônica de mesa, com 12 dígitos, alimentação com bateria HR1130 ou célula solar. Marca: Kenko.</t>
+          <t>EXTRATOR DE GRAMPO, MATERIAL: AÇO, TIPO: ESPATULA. MARCA: FERSAN</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="E33" t="n">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
@@ -1510,17 +1510,17 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E35" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
@@ -1558,7 +1558,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>30.16.2252</t>
+          <t>30.16.2250</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1568,21 +1568,21 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>FITA SINALIZAÇÃO, MATERIAL PLÁSTICO, COMPRIMENTO 180M OU SUPERIOR, LARGURA 70MM, COR PRETA E AMARELA, APLICAÇÃO SINALIZAÇÃO DE ADVERTÊNCIA, CARACTERÍSTICAS ADICIONAIS FORMATO CORES EM DIAGONAL, ZEBRADA.</t>
+          <t>FITA ADESIVA, MATERIAL PROPILENO OU POLIPROPILENO, TRANSPARENTE, MONOFACE, LARGURA 25MM, COMPRIMENTO 50M, INCOLOR.</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="E37" t="n">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F37" t="n">
-        <v>-54</v>
+        <v>0</v>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
@@ -1761,14 +1761,14 @@
         <v>159</v>
       </c>
       <c r="E43" t="n">
-        <v>159</v>
+        <v>14</v>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
@@ -1823,21 +1823,21 @@
         <v>97</v>
       </c>
       <c r="E45" t="n">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F45" t="n">
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>30.16.2291</t>
+          <t>30.16.2352</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1847,14 +1847,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>CANETA MARCA-TEXTO, MATERIAL PLÁSTICO, TIPO PONTA FLUORESCENTE, COR AZUL.</t>
+          <t>GRAMPO GRAMPEADOR, MATERIAL METAL, TAMANHO 23/20.</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E46" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1868,7 +1868,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>30.16.2352</t>
+          <t>30.16.2353</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1878,28 +1878,28 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>GRAMPO GRAMPEADOR, MATERIAL METAL, TAMANHO 23/20.</t>
+          <t>GRAMPO GRAMPEADOR, MATERIAL METAL, TAMANHO 23/13.</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E47" t="n">
         <v>23</v>
       </c>
       <c r="F47" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>30.16.2353</t>
+          <t>30.16.2357</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1909,17 +1909,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>GRAMPO GRAMPEADOR, MATERIAL METAL, TAMANHO 23/13.</t>
+          <t>CAIXA ARQUIVO, MATERIAL PLÁSTICO, 135 X 250 X 360MM, CORES VARIADAS.</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E48" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
@@ -1930,7 +1930,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>30.16.2357</t>
+          <t>30.16.2362</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1940,28 +1940,28 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>CAIXA ARQUIVO, MATERIAL PLÁSTICO, 135 X 250 X 360MM, CORES VARIADAS.</t>
+          <t>FITA ADESIVA, MATERIAL CELOFANE TRANSPARENTE, MONOFACE, LARGURA 12mm, COMPRIMENTO 50m, INCOLOR. MARCA: ADELBRAS.</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E49" t="n">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="F49" t="n">
-        <v>5</v>
+        <v>-45</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>pedido no suap</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>30.16.2360</t>
+          <t>30.16.2378</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1971,28 +1971,28 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>FITA ADESIVA, MATERIAL POLIPROPILENO TRANSPARENTE, TIPO MONOFACE, LARGURA 25mm, COMPRIMENTO 50m, INCOLOR. MARCA: ADELBRAS.</t>
+          <t>PASTA ARQUIVO, MATERIAL CARTÃO PRENSADO PLASTIFICADO, TIPO AZ, LOMBADA LARGA, APLICAÇÃO ARQUIVO.</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>13</v>
+        <v>128</v>
       </c>
       <c r="E50" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F50" t="n">
-        <v>-54</v>
+        <v>62</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>30.16.2362</t>
+          <t>30.16.2383</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2002,28 +2002,28 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>FITA ADESIVA, MATERIAL CELOFANE TRANSPARENTE, MONOFACE, LARGURA 12mm, COMPRIMENTO 50m, INCOLOR. MARCA: ADELBRAS.</t>
+          <t>PAPEL EMBORRACHADO, MATERIAL BORRACHA EVA, COMPRIMENTO 60 cm, LARGURA 40 cm, ESPESSURA 2mm, PADRÃO LISO, CORES VARIADAS.</t>
         </is>
       </c>
       <c r="D51" t="n">
+        <v>19</v>
+      </c>
+      <c r="E51" t="n">
         <v>6</v>
       </c>
-      <c r="E51" t="n">
-        <v>51</v>
-      </c>
       <c r="F51" t="n">
-        <v>-45</v>
+        <v>13</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>30.16.2378</t>
+          <t>30.16.2432</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2033,28 +2033,28 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>PASTA ARQUIVO, MATERIAL CARTÃO PRENSADO PLASTIFICADO, TIPO AZ, LOMBADA LARGA, APLICAÇÃO ARQUIVO.</t>
+          <t>PINCEL MARCADOR PERMANENTE CD, MATERIAL PLÁSTICO RECICLADO, TIPO PONTA FELTRO, COR TINTA VARIADA. MARCA: BRW.</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>128</v>
+        <v>18</v>
       </c>
       <c r="E52" t="n">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="F52" t="n">
-        <v>18</v>
+        <v>-19</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>pedido no suap</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>30.16.2383</t>
+          <t>30.16.2477</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2064,28 +2064,28 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>PAPEL EMBORRACHADO, MATERIAL BORRACHA EVA, COMPRIMENTO 60 cm, LARGURA 40 cm, ESPESSURA 2mm, PADRÃO LISO, CORES VARIADAS.</t>
+          <t>PERFURADOR DE PAPEL, MATERIAL METAL, TIPO GRANDE, TRATAMENTO SUPERFICIAL NIQUELADO, CAPACIDADE PERFURAÇÃO 20 FL, FUNCIONAMENTO MANUAL.</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>pedido no suap</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>30.16.2384</t>
+          <t>30.16.2484</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2095,28 +2095,28 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>PAPEL CELOFANE, COMPRIMENTO 100 cm, LARGURA 85 cm, CORES VARIADAS, APLICAÇÃO TRABALHADO EDUCATIVOS, GRAMATURA 18 G/M2.</t>
+          <t>TNT, GRAMATURA 100 G/M2, COR BRANCA, LARGURA 1,40 M.</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E54" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F54" t="n">
-        <v>-7</v>
+        <v>29</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>30.16.2426</t>
+          <t>30.16.2531</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2126,28 +2126,28 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>ENVELOPE MATERIAL PAPEL KRAFT, GRAMATURA 90G/M², COMPRIMENTO 410 mm, LARGURA 310 mm.</t>
+          <t>GRAMPO GRAMPEADOR, MATERIAL AÇO, TRATAMENTO SUPERFICIAL NIQUELADO, TAMANHO 26/6.</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="E55" t="n">
-        <v>171</v>
+        <v>8</v>
       </c>
       <c r="F55" t="n">
-        <v>-55</v>
+        <v>0</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>30.16.2432</t>
+          <t>30.16.2532</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2157,28 +2157,28 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>PINCEL MARCADOR PERMANENTE CD, MATERIAL PLÁSTICO RECICLADO, TIPO PONTA FELTRO, COR TINTA VARIADA. MARCA: BRW.</t>
+          <t>GRAMPEADOR, MATERIAL METAL, TIPO MESA, CAPACIDADE 100 FL, TAMANHO GRAMPO 23/6 A 23/23.</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E56" t="n">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="F56" t="n">
-        <v>-19</v>
+        <v>0</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>30.16.2477</t>
+          <t>30.16.2533</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2188,14 +2188,14 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>PERFURADOR DE PAPEL, MATERIAL METAL, TIPO GRANDE, TRATAMENTO SUPERFICIAL NIQUELADO, CAPACIDADE PERFURAÇÃO 20 FL, FUNCIONAMENTO MANUAL.</t>
+          <t>CANETA ESFEROGRÁFICA, MATERIAL PLÁSTICO, COR PRETA, MATERIAL TRANSPARENTE. MARCA: BIC.</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>1</v>
+        <v>313</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
+        <v>313</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
@@ -2209,7 +2209,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>30.16.2531</t>
+          <t>30.16.2534</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2219,28 +2219,28 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>GRAMPO GRAMPEADOR, MATERIAL AÇO, TRATAMENTO SUPERFICIAL NIQUELADO, TAMANHO 26/6.</t>
+          <t>CANETA ESFEROGRÁFICA, MATERIAL PLÁSTICO, COR AZUL, MATERIAL TRANSPARENTE. MARCA: BIC.</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>8</v>
+        <v>526</v>
       </c>
       <c r="E58" t="n">
-        <v>27</v>
+        <v>378</v>
       </c>
       <c r="F58" t="n">
-        <v>-19</v>
+        <v>148</v>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>30.16.2532</t>
+          <t>30.16.2535</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2250,28 +2250,28 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>GRAMPEADOR, MATERIAL METAL, TIPO MESA, CAPACIDADE 100 FL, TAMANHO GRAMPO 23/6 A 23/23.</t>
+          <t>CANETA ESFEROGRÁFICA, MATERIAL PLÁSTICO, COR VERMELHA, MATERIAL TRANSPARENTE. MARCA: BIC.</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="E59" t="n">
-        <v>10</v>
+        <v>196</v>
       </c>
       <c r="F59" t="n">
-        <v>0</v>
+        <v>-141</v>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>30.16.2534</t>
+          <t>30.16.2540</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2281,28 +2281,28 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CANETA ESFEROGRÁFICA, MATERIAL PLÁSTICO, COR AZUL, MATERIAL TRANSPARENTE. MARCA: BIC.</t>
+          <t>PORTA-FITA ADESIVA, MATERIAL PLÁSTICO, COR PRETA, COMPRIMENTO 21 CM, LARGURA 9 CM, CARACTERÍSTICAS ADICIONAIS COM CORTADOR FITA DE METAL E BASE ANTIDERRAPANTE.</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>536</v>
+        <v>13</v>
       </c>
       <c r="E60" t="n">
-        <v>391</v>
+        <v>13</v>
       </c>
       <c r="F60" t="n">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>pedido no suap</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>30.16.2540</t>
+          <t>30.16.2563</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2312,28 +2312,28 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>PORTA-FITA ADESIVA, MATERIAL PLÁSTICO, COR PRETA, COMPRIMENTO 21 CM, LARGURA 9 CM, CARACTERÍSTICAS ADICIONAIS COM CORTADOR FITA DE METAL E BASE ANTIDERRAPANTE.</t>
+          <t>PASTA ARQUIVO, MATERIAL PVC, TIPO SANFONADA, LARGURA 280 MM, ALTURA 390 MM, COR INCOLOR, CARACTERÍSTICAS ADICIONAIS ELÁSTICO, 31 DIVISÓRIAS, VISOR E ETIQUETA.</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E61" t="n">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
+        <v>-29</v>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>30.16.2563</t>
+          <t>30.16.2566</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2343,17 +2343,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>PASTA ARQUIVO, MATERIAL PVC, TIPO SANFONADA, LARGURA 280 MM, ALTURA 390 MM, COR INCOLOR, CARACTERÍSTICAS ADICIONAIS ELÁSTICO, 31 DIVISÓRIAS, VISOR E ETIQUETA.</t>
+          <t>PASTA ARQUIVO, MATERIAL CARTÃO PLASTIFICADO, LOMBADA 20 MM, COR AZUL, CARACTERÍSTICAS ADICIONAIS COM ABA E ELÁSTICO, TAMANHO OFÍCIO</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E62" t="n">
-        <v>54</v>
+        <v>170</v>
       </c>
       <c r="F62" t="n">
-        <v>-30</v>
+        <v>-137</v>
       </c>
       <c r="G62" t="inlineStr">
         <is>
@@ -2364,7 +2364,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>30.16.2566</t>
+          <t>30.16.2567</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2378,13 +2378,13 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="E63" t="n">
-        <v>340</v>
+        <v>413</v>
       </c>
       <c r="F63" t="n">
-        <v>-307</v>
+        <v>-356</v>
       </c>
       <c r="G63" t="inlineStr">
         <is>
@@ -2395,7 +2395,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>30.16.2567</t>
+          <t>30.16.2572</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2405,17 +2405,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>PASTA ARQUIVO, MATERIAL CARTÃO PLASTIFICADO, LOMBADA 20 MM, COR AZUL, CARACTERÍSTICAS ADICIONAIS COM ABA E ELÁSTICO, TAMANHO OFÍCIO</t>
+          <t>PRENDEDOR PAPEL, MATERIAL METAL, TIPO MOLA, TAMANHO MOLA 41 MM</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="E64" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F64" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G64" t="inlineStr">
         <is>
@@ -2426,7 +2426,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>30.16.2572</t>
+          <t>30.16.2574</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2436,14 +2436,14 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>PRENDEDOR PAPEL, MATERIAL METAL, TIPO MOLA, TAMANHO MOLA 41 MM</t>
+          <t>CONJUNTO MULTIUSO ESCRITÓRIO, MATERIAL ACRÍLICO, APLICAÇÃO LÁPIS, ACESSÓRIOS REGUA, TESOURA, LAPIS, CANETA, BORRACHA,_ESQUADRO, MODELO BÁSICO.</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="E65" t="n">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="F65" t="n">
         <v>0</v>
@@ -2457,7 +2457,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>30.16.2573</t>
+          <t>30.16.2594</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2467,17 +2467,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CAIXA CORRESPONDÊNCIA, MATERIAL ACRÍLICO, COR FUMÊ, TIPO TRIPLA, COMPRIMENTO 370 MM, LARGURA 260 MM, ALTURA 50 MM, CARACTERÍSTICAS ADICIONAIS ARTICULAÇÃO EM ACRÍLICO</t>
+          <t>LIVRO PROTOCOLO, QUANTIDADE FOLHAS 100 UN, COMPRIMENTO 220 MM, LARGURA 155 MM,TIPO CAPA DURA, CARACTERÍSTICAS ADICIONAIS IMPRESSÃO OFSETE, DUAS FACES, COR PRETA, MATERIAL CAPA PAPELÃO, GRAMATURA FOLHAS 75 G/M2, MATERIAL FOLHAS PAPEL APERGAMINHADO</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="E66" t="n">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="F66" t="n">
-        <v>-11</v>
+        <v>-20</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
@@ -2488,7 +2488,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>30.16.2574</t>
+          <t>30.16.2667</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2498,28 +2498,28 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CONJUNTO MULTIUSO ESCRITÓRIO, MATERIAL ACRÍLICO, APLICAÇÃO LÁPIS, ACESSÓRIOS REGUA, TESOURA, LAPIS, CANETA, BORRACHA,_ESQUADRO, MODELO BÁSICO.</t>
+          <t>PAPEL CARTOLINA , MATERIAL CELULOSE VEGETAL, GRAMATURA 180 G/M2, CORES: DIVERSAS.</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="E67" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F67" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>30.16.2591</t>
+          <t>30.16.2669</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2529,28 +2529,28 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>PINCEL MARCADOR PERMANENTE CD, MATERIAL PLÁSTICO RECICLADO, TIPO PONTA FELTRO,COR TINTA VARIADA</t>
+          <t>PAPEL SULFITE, PACOTE COM 100 FOLHAS.</t>
         </is>
       </c>
       <c r="D68" t="n">
+        <v>3</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F68" t="n">
         <v>2</v>
       </c>
-      <c r="E68" t="n">
-        <v>11</v>
-      </c>
-      <c r="F68" t="n">
-        <v>-9</v>
-      </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>30.16.2594</t>
+          <t>30.16.362</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2560,17 +2560,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>LIVRO PROTOCOLO, QUANTIDADE FOLHAS 100 UN, COMPRIMENTO 220 MM, LARGURA 155 MM,TIPO CAPA DURA, CARACTERÍSTICAS ADICIONAIS IMPRESSÃO OFSETE, DUAS FACES, COR PRETA, MATERIAL CAPA PAPELÃO, GRAMATURA FOLHAS 75 G/M2, MATERIAL FOLHAS PAPEL APERGAMINHADO</t>
+          <t>COLCHETE (BAILARINA), Nº 12, COMPRIMENTO DA HASTE 6,3CM, DIÂMETRO DA CABEÇA 14MM, PARA FIXAR ATÉ 270 FOLHAS, MATERIAL LATÃO, CAIXA COM 72 UNIDADES.</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="E69" t="n">
-        <v>94</v>
+        <v>6</v>
       </c>
       <c r="F69" t="n">
-        <v>-20</v>
+        <v>-2</v>
       </c>
       <c r="G69" t="inlineStr">
         <is>
@@ -2581,7 +2581,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>30.16.2667</t>
+          <t>30.16.684</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2591,17 +2591,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>PAPEL CARTOLINA , MATERIAL CELULOSE VEGETAL, GRAMATURA 180 G/M2, CORES: DIVERSAS.</t>
+          <t>CLIPE II - TAMANHO 8/0, CAIXA COM 25 UN</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="E70" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="F70" t="n">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
@@ -2612,58 +2612,58 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>30.16.2669</t>
+          <t>30.17.350</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>16 - MATERIAL DE EXPEDIENTE</t>
+          <t>17 - MATERIAL DE PROCESSAMENTO DE DADOS</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>PAPEL SULFITE, PACOTE COM 100 FOLHAS.</t>
+          <t>CD-R - DISCO LASER, GRAVÁVEL, 700 MB, 80 MIN.</t>
         </is>
       </c>
       <c r="D71" t="n">
+        <v>33</v>
+      </c>
+      <c r="E71" t="n">
+        <v>30</v>
+      </c>
+      <c r="F71" t="n">
         <v>3</v>
       </c>
-      <c r="E71" t="n">
-        <v>3</v>
-      </c>
-      <c r="F71" t="n">
-        <v>0</v>
-      </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>30.16.362</t>
+          <t>30.17.519</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>16 - MATERIAL DE EXPEDIENTE</t>
+          <t>17 - MATERIAL DE PROCESSAMENTO DE DADOS</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>COLCHETE (BAILARINA), Nº 12, COMPRIMENTO DA HASTE 6,3CM, DIÂMETRO DA CABEÇA 14MM, PARA FIXAR ATÉ 270 FOLHAS, MATERIAL LATÃO, CAIXA COM 72 UNIDADES.</t>
+          <t>DVD-R, CAPACIDADE 4,7GB, TIPO GRAVÁVEL, MONOFACE</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="E72" t="n">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="F72" t="n">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
@@ -2674,86 +2674,86 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>30.16.45</t>
+          <t>30.17.789</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>16 - MATERIAL DE EXPEDIENTE</t>
+          <t>17 - MATERIAL DE PROCESSAMENTO DE DADOS</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>EXTRATOR DE GRAMPO</t>
+          <t>SUPORTE FIXAÇÃO PROJETOR, MATERIAL FERRO, FORMATO DISCO, TIPO UNIVERSAL.</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E73" t="n">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="F73" t="n">
-        <v>-39</v>
+        <v>0</v>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>30.16.490</t>
+          <t>30.19.224</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16 - MATERIAL DE EXPEDIENTE</t>
+          <t>19 - MATERIAL DE ACONDICIONAMENTO E EMBALAGEM</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>LÁPIS PRETO, CORPO DE MADEIRA, DIÂMETRO CARGA 2MM, DUREZA HB, FORMATO CORPO CILÍNDRICO, SEM BORRACHA APAGADORA, GRAFITE Nº2, MATERIAL CARGA GRAFITE</t>
+          <t>FILME PVC/PLÁSTICO, ESTIRÁVEL, DIMENSÕES 10CMX100M.</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E74" t="n">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="F74" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>30.16.684</t>
+          <t>30.22.500</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16 - MATERIAL DE EXPEDIENTE</t>
+          <t>22 - MATERIAL DE LIMPEZA E PROD. DE HIGIENIZACAO</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>CLIPE II - TAMANHO 8/0, CAIXA COM 25 UN</t>
+          <t>PÁ COLETORA DE LIXO C/ MOVIMENTO BASCULANTE DA CAIXA DE RECOLHIMENTO</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E75" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
@@ -2767,24 +2767,24 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>30.16.966</t>
+          <t>30.24.110</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>16 - MATERIAL DE EXPEDIENTE</t>
+          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>TINTA PARA CARIMBO (AZUL) COMPONENTES ÁGUA, PIGMENTOS, ASPECTO FÍSICO LÍQUIDO,FRASCO COM 40 ML</t>
+          <t>SIFÃO SANFONADO SIMPLES (C/SAÍDA DE 40MM)</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E76" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F76" t="n">
         <v>0</v>
@@ -2798,24 +2798,24 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>30.17.350</t>
+          <t>30.24.1816</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>17 - MATERIAL DE PROCESSAMENTO DE DADOS</t>
+          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>CD-R - DISCO LASER, GRAVÁVEL, 700 MB, 80 MIN.</t>
+          <t>FITA VEDA ROSCA 50M X 18MM, ESPESSURA 0,06 A 0,08MM</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E77" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F77" t="n">
         <v>3</v>
@@ -2829,148 +2829,148 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>30.17.519</t>
+          <t>30.24.2055</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>17 - MATERIAL DE PROCESSAMENTO DE DADOS</t>
+          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>DVD-R, CAPACIDADE 4,7GB, TIPO GRAVÁVEL, MONOFACE</t>
+          <t>FECHADURA MATERIAL CAIXA AÇO INOXIDÁVEL MARCA SOPRANO.</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="E78" t="n">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="F78" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>30.17.789</t>
+          <t>30.24.2646</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>17 - MATERIAL DE PROCESSAMENTO DE DADOS</t>
+          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>SUPORTE FIXAÇÃO PROJETOR, MATERIAL FERRO, FORMATO DISCO, TIPO UNIVERSAL.</t>
+          <t>TORNEIRA, MATERIAL CORPO METAL, TIPO PIA, 3/4 POL, ACABAMENTO SUPERFICIAL CROMADO, LONGA</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E79" t="n">
         <v>8</v>
       </c>
       <c r="F79" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>30.22.500</t>
+          <t>30.24.2722</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>22 - MATERIAL DE LIMPEZA E PROD. DE HIGIENIZACAO</t>
+          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>PÁ COLETORA DE LIXO C/ MOVIMENTO BASCULANTE DA CAIXA DE RECOLHIMENTO</t>
+          <t>CHUVEIRO NÃO ELETRICO, MATERIAL PVC, TIPO COM BRAÇO, SEM REGISTRO, COR BRANCA, BITOLA 1/2 POL</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E80" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F80" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>30.22.653</t>
+          <t>30.24.2910</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>22 - MATERIAL DE LIMPEZA E PROD. DE HIGIENIZACAO</t>
+          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>DISPENSER PARA PAPEL TOALHA, INTERFOLHADO. CARACT.: PAPELEIRA PARA PAPEL TOALHA. INTERFOLHA: 2 OU 3 DOBRAS. CAPACIDADE: PACOTE 1.000 FLS. MARCA: BELLPLUS.</t>
+          <t>CONEXÃO HIDRÁULICA LUVA PVC 25MM LISA.</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E81" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F81" t="n">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>30.22.688</t>
+          <t>30.24.3223</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>22 - MATERIAL DE LIMPEZA E PROD. DE HIGIENIZACAO</t>
+          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>CONJUNTO LIXEIRA SELETIVA COM 4 UNIDADES, 50L, CORES AZUL, VERMELHA, VERDE E AMARELA.</t>
+          <t>Adesivo conexao hidraulica composicao acetona metilcetona tolual e resina PVC, przo de validade 1 ano apos fabricacao, aplicacao tubos e conexoes de pvc, apresentacao tubo de 75 GR</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F82" t="n">
         <v>0</v>
@@ -2984,55 +2984,55 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>30.22.695</t>
+          <t>30.24.3281</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>22 - MATERIAL DE LIMPEZA E PROD. DE HIGIENIZACAO</t>
+          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>VASSOURA JARDINAGEM, TIPO FIXA, MATERIAL CERDAS PALHA, TIPO LÂMINA CHATA, COM CABO.</t>
+          <t>Parafuso de Fenda Phillips Cabeça Chata com Bucha Universal de 10mm</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="F83" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>pedido no suap</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>30.24.110</t>
+          <t>30.26.1190</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
+          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>SIFÃO SANFONADO SIMPLES (C/SAÍDA DE 40MM)</t>
+          <t>CABO ELÉTRICO, UNIPOLAR, FLEXÍVEL, COBRE, 4MM, 750V, PRETO</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E84" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F84" t="n">
         <v>0</v>
@@ -3046,55 +3046,55 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>30.24.1816</t>
+          <t>30.26.1280</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
+          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>FITA VEDA ROSCA 50M X 18MM, ESPESSURA 0,06 A 0,08MM</t>
+          <t>DISJUNTOR BAIXA TENSÃO, TERMOMAGNÉTICO, 1 POLO, 25A, 220V.</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="E85" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="F85" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>pedido no suap</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>30.24.2055</t>
+          <t>30.26.1410</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
+          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>FECHADURA MATERIAL CAIXA AÇO INOXIDÁVEL MARCA SOPRANO.</t>
+          <t>30.26.1409 CABO ELETRICO FLEXIVEL, MATERIAL COBRE ELETROLITICO, REVESTIMENTO PVC. TEMPERATURA 70ºC. TENSÃO ISOLAMENTO 750 V, COR VERDE, SEÇÃO NOMINAL CONDUTOR 4MM2, BITOLA CONDUTOR 4 MM2, QUANTIDADES FIO 1</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E86" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F86" t="n">
         <v>0</v>
@@ -3108,55 +3108,55 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>30.24.2646</t>
+          <t>30.26.194</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
+          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>TORNEIRA, MATERIAL CORPO METAL, TIPO PIA, 3/4 POL, ACABAMENTO SUPERFICIAL CROMADO, LONGA</t>
+          <t>CABO ELÉTRICO - 2,5 MM², COR PRETO , FLEXIVEL.</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E87" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>pedido no suap</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>30.24.2722</t>
+          <t>30.26.2480</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
+          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>CHUVEIRO NÃO ELETRICO, MATERIAL PVC, TIPO COM BRAÇO, SEM REGISTRO, COR BRANCA, BITOLA 1/2 POL</t>
+          <t>CABO VGA - MACHO / MACHO - COMPRIMENTO 10 METROS.</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E88" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -3170,100 +3170,100 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>30.24.2910</t>
+          <t>30.26.25</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
+          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>CONEXÃO HIDRÁULICA LUVA PVC 25MM LISA.</t>
+          <t>CABO ELÉTRICO, UNIPOLAR, FLEXÍVEL, COBRE, 2,5MM, 750V, VERDE</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E89" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F89" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>pedido no suap</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>30.24.3223</t>
+          <t>30.26.2898</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
+          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Adesivo conexao hidraulica composicao acetona metilcetona tolual e resina PVC, przo de validade 1 ano apos fabricacao, aplicacao tubos e conexoes de pvc, apresentacao tubo de 75 GR</t>
+          <t>Cabo Elétrico Flexível, 4MM, Cobre, 750V, Amarelo.</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E90" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F90" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>saida sem pedido</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>30.24.3281</t>
+          <t>30.26.2899</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>24 - MATERIAL P/ MANUT.DE BENS IMOVEIS/INSTALACOES</t>
+          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Parafuso de Fenda Phillips Cabeça Chata com Bucha Universal de 10mm</t>
+          <t>Cabo Elétrico Flexível, 2,5MM, Cobre, 750V, Azul.</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>98</v>
+        <v>3</v>
       </c>
       <c r="E91" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="F91" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>pedido no suap</t>
+          <t>adequado</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>30.26.1190</t>
+          <t>30.26.3102</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -3273,28 +3273,28 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>CABO ELÉTRICO, UNIPOLAR, FLEXÍVEL, COBRE, 4MM, 750V, PRETO</t>
+          <t>TOMADA, MODELO PLUGUE, TIPO FÊMEA, FORMATO CONTATO PINO CILÍNDRICO, CORRENTE NOMINAL 20 A, TENSÃO NOMINAL 250 V, NÚMERO PÓLOS 2 P + T</t>
         </is>
       </c>
       <c r="D92" t="n">
         <v>1</v>
       </c>
       <c r="E92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F92" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>30.26.1280</t>
+          <t>30.26.429</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -3304,14 +3304,14 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>DISJUNTOR BAIXA TENSÃO, TERMOMAGNÉTICO, 1 POLO, 25A, 220V.</t>
+          <t>SOQUETE LÂMPADA FLUORESCENTE, TIPO ANTIVIBRATÓRIO, 40W, TENSÃO 220V.</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F93" t="n">
         <v>0</v>
@@ -3325,55 +3325,55 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>30.26.1410</t>
+          <t>30.28.350</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
+          <t>28 - MATERIAL DE PROTECAO E SEGURANCA</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>30.26.1409 CABO ELETRICO FLEXIVEL, MATERIAL COBRE ELETROLITICO, REVESTIMENTO PVC. TEMPERATURA 70ºC. TENSÃO ISOLAMENTO 750 V, COR VERDE, SEÇÃO NOMINAL CONDUTOR 4MM2, BITOLA CONDUTOR 4 MM2, QUANTIDADES FIO 1</t>
+          <t>ras reutilizáveis, com 03 (tres) camadas de tecido: uma camada de tecido não impermeável na parte frontal, tecido respirável no meio e algodão na parte em contato com a superfície do rosto. Algodao (anatomicas). COM LOGOMARCA DO ORGAO. ABNT PR 1002</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>2</v>
+        <v>1440</v>
       </c>
       <c r="E94" t="n">
-        <v>2</v>
+        <v>2200</v>
       </c>
       <c r="F94" t="n">
-        <v>0</v>
+        <v>-760</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>adequado</t>
+          <t>saida sem pedido</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>30.26.194</t>
+          <t>30.36.473</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
+          <t>36 - MATERIAL HOSPITALAR</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>CABO ELÉTRICO - 2,5 MM², COR PRETO , FLEXIVEL.</t>
+          <t>DISPENSER PAPEL TOALHA, MATERIAL AÇO, TIPO INTERFOLHA, COR BRANCA, COM CHAVE.</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E95" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F95" t="n">
         <v>0</v>
@@ -3387,370 +3387,29 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>30.26.2480</t>
+          <t>30.36.489</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
+          <t>36 - MATERIAL HOSPITALAR</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>CABO VGA - MACHO / MACHO - COMPRIMENTO 10 METROS.</t>
+          <t>TERMÔMETRO, TIPO DIGITAL COM ALARME, VISOR EM CRISTAL LÍQUIDO, MEDIÇÃO TEMPERATURA 40 A 95 ºC, APLICAÇÃO ALIMENTOS, MATERIAL PLÁSTICO, À PROVA D'ÁGUA, BATERIA/PILHA.</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E96" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
       </c>
       <c r="G96" t="inlineStr">
-        <is>
-          <t>adequado</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>30.26.25</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>CABO ELÉTRICO, UNIPOLAR, FLEXÍVEL, COBRE, 2,5MM, 750V, VERDE</t>
-        </is>
-      </c>
-      <c r="D97" t="n">
-        <v>3</v>
-      </c>
-      <c r="E97" t="n">
-        <v>3</v>
-      </c>
-      <c r="F97" t="n">
-        <v>0</v>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>adequado</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>30.26.2898</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>Cabo Elétrico Flexível, 4MM, Cobre, 750V, Amarelo.</t>
-        </is>
-      </c>
-      <c r="D98" t="n">
-        <v>2</v>
-      </c>
-      <c r="E98" t="n">
-        <v>2</v>
-      </c>
-      <c r="F98" t="n">
-        <v>0</v>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>adequado</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>30.26.2899</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>Cabo Elétrico Flexível, 2,5MM, Cobre, 750V, Azul.</t>
-        </is>
-      </c>
-      <c r="D99" t="n">
-        <v>3</v>
-      </c>
-      <c r="E99" t="n">
-        <v>3</v>
-      </c>
-      <c r="F99" t="n">
-        <v>0</v>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>adequado</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>30.26.429</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>26 - MATERIAL ELETRICO E ELETRONICO</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>SOQUETE LÂMPADA FLUORESCENTE, TIPO ANTIVIBRATÓRIO, 40W, TENSÃO 220V.</t>
-        </is>
-      </c>
-      <c r="D100" t="n">
-        <v>50</v>
-      </c>
-      <c r="E100" t="n">
-        <v>50</v>
-      </c>
-      <c r="F100" t="n">
-        <v>0</v>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>adequado</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>30.28.344</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>28 - MATERIAL DE PROTECAO E SEGURANCA</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>Máscara multiuso, poliéster e algodão, uso reutilizável, proteção individual, tripla camada, com elástico.</t>
-        </is>
-      </c>
-      <c r="D101" t="n">
-        <v>817</v>
-      </c>
-      <c r="E101" t="n">
-        <v>16</v>
-      </c>
-      <c r="F101" t="n">
-        <v>801</v>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>pedido no suap</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>30.28.350</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>28 - MATERIAL DE PROTECAO E SEGURANCA</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>ras reutilizáveis, com 03 (tres) camadas de tecido: uma camada de tecido não impermeável na parte frontal, tecido respirável no meio e algodão na parte em contato com a superfície do rosto. Algodao (anatomicas). COM LOGOMARCA DO ORGAO. ABNT PR 1002</t>
-        </is>
-      </c>
-      <c r="D102" t="n">
-        <v>1440</v>
-      </c>
-      <c r="E102" t="n">
-        <v>6300</v>
-      </c>
-      <c r="F102" t="n">
-        <v>-4860</v>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>saida sem pedido</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>30.36.466</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>36 - MATERIAL HOSPITALAR</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>SACO PLÁSTICO LIXO, CAPACIDADE 30 L, COR BRANCO LEITOSO, LARGURA 59 CM, ALTURA 2 CM, APLICAÇÃO HOSPITALAR, MATERIAL POLIETILENO ALTA DENSIDADE.</t>
-        </is>
-      </c>
-      <c r="D103" t="n">
-        <v>1200</v>
-      </c>
-      <c r="E103" t="n">
-        <v>22</v>
-      </c>
-      <c r="F103" t="n">
-        <v>1178</v>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>pedido no suap</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>30.36.467</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>36 - MATERIAL HOSPITALAR</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>DISPENSER HIGIENIZADOR, MATERIAL ACRÍLICO, CAPACIDADE 800 ML, TIPO FIXAÇÃO PAREDE, COR TRANSPARENTE, APLICAÇÃO MÃOS.</t>
-        </is>
-      </c>
-      <c r="D104" t="n">
-        <v>1</v>
-      </c>
-      <c r="E104" t="n">
-        <v>1</v>
-      </c>
-      <c r="F104" t="n">
-        <v>0</v>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>adequado</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>30.36.470</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>36 - MATERIAL HOSPITALAR</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>BOMBONA, MATERIAL PLÁSTICO, CAPACIDADE 5 L, APLICAÇÃO LABORATÓRIO, COM TAMPA.</t>
-        </is>
-      </c>
-      <c r="D105" t="n">
-        <v>20</v>
-      </c>
-      <c r="E105" t="n">
-        <v>20</v>
-      </c>
-      <c r="F105" t="n">
-        <v>0</v>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>adequado</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>30.36.473</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>36 - MATERIAL HOSPITALAR</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>DISPENSER PAPEL TOALHA, MATERIAL AÇO, TIPO INTERFOLHA, COR BRANCA, COM CHAVE.</t>
-        </is>
-      </c>
-      <c r="D106" t="n">
-        <v>9</v>
-      </c>
-      <c r="E106" t="n">
-        <v>9</v>
-      </c>
-      <c r="F106" t="n">
-        <v>0</v>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>adequado</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>30.36.489</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>36 - MATERIAL HOSPITALAR</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>TERMÔMETRO, TIPO DIGITAL COM ALARME, VISOR EM CRISTAL LÍQUIDO, MEDIÇÃO TEMPERATURA 40 A 95 ºC, APLICAÇÃO ALIMENTOS, MATERIAL PLÁSTICO, À PROVA D'ÁGUA, BATERIA/PILHA.</t>
-        </is>
-      </c>
-      <c r="D107" t="n">
-        <v>7</v>
-      </c>
-      <c r="E107" t="n">
-        <v>7</v>
-      </c>
-      <c r="F107" t="n">
-        <v>0</v>
-      </c>
-      <c r="G107" t="inlineStr">
         <is>
           <t>adequado</t>
         </is>

</xml_diff>